<commit_message>
implemented duckduckgo libary for searching
</commit_message>
<xml_diff>
--- a/testing/output/test_data.xlsx
+++ b/testing/output/test_data.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="TestFinancials" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BalanceSheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CashFlow" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +444,16 @@
           <t>2025E</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Updated</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>2026E</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,6 +470,12 @@
       <c r="D2" t="n">
         <v>1440000</v>
       </c>
+      <c r="E2" t="n">
+        <v>1600000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1800000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -521,6 +539,195 @@
       </c>
       <c r="D6" t="n">
         <v>360000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Accounts Receivable</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Total Assets</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>500000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Debt</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>200000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Equity</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>300000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>350000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Operating CF</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>120000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Investing CF</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-80000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Financing CF</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-20000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Net Change in Cash</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>